<commit_message>
updated training_lhs.xlsx for measure resources
</commit_message>
<xml_diff>
--- a/projects/training_lhs.xlsx
+++ b/projects/training_lhs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="0" windowWidth="16800" windowHeight="12816" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="16800" yWindow="0" windowWidth="2964" windowHeight="9108" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="702">
   <si>
     <t>type</t>
   </si>
@@ -2045,15 +2045,6 @@
   </si>
   <si>
     <t>AedgOfficeHvacVavDx</t>
-  </si>
-  <si>
-    <t>This space type should be part of a ceiling return air plenum.</t>
-  </si>
-  <si>
-    <t>ceilingReturnPlenumSpaceType</t>
-  </si>
-  <si>
-    <t>|</t>
   </si>
   <si>
     <t>Total Cost for HVAC System ($).</t>
@@ -5558,8 +5549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6082,10 +6073,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z96"/>
+  <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6283,10 +6274,10 @@
         <v>645</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>72</v>
@@ -6776,7 +6767,7 @@
         <v>652</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>653</v>
@@ -6859,7 +6850,7 @@
         <v>23</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E34" s="34" t="s">
         <v>132</v>
@@ -6882,7 +6873,7 @@
         <v>173</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>174</v>
@@ -6971,7 +6962,7 @@
         <v>66</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3">
@@ -6982,7 +6973,7 @@
         <v>173</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>174</v>
@@ -7071,7 +7062,7 @@
         <v>66</v>
       </c>
       <c r="J44" s="34" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3">
@@ -7082,7 +7073,7 @@
         <v>173</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>174</v>
@@ -7171,12 +7162,12 @@
         <v>66</v>
       </c>
       <c r="J49" s="34" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="50" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B50" s="34" t="s">
         <v>665</v>
@@ -7205,10 +7196,10 @@
         <v>2</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="J51" s="34" t="s">
-        <v>670</v>
+        <v>68</v>
+      </c>
+      <c r="I51" s="34">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.3">
@@ -7216,40 +7207,35 @@
         <v>23</v>
       </c>
       <c r="D52" s="34" t="s">
+        <v>670</v>
+      </c>
+      <c r="E52" s="34" t="s">
         <v>671</v>
       </c>
-      <c r="E52" s="34" t="s">
-        <v>672</v>
-      </c>
       <c r="F52" s="34" t="s">
         <v>2</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="I52" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>673</v>
-      </c>
-      <c r="E53" s="34" t="s">
-        <v>674</v>
-      </c>
-      <c r="F53" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="G53" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I53" s="34" t="b">
+      <c r="I52" s="34" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="53" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
@@ -7264,10 +7250,15 @@
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
       <c r="R54" s="1"/>
+      <c r="T54" s="1"/>
     </row>
     <row r="55" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -7279,15 +7270,20 @@
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
+      <c r="P55" s="26"/>
+      <c r="Q55" s="26"/>
       <c r="R55" s="1"/>
-      <c r="T55" s="1"/>
+      <c r="S55" s="26"/>
+      <c r="T55" s="26"/>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="26"/>
     </row>
     <row r="56" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -7299,7 +7295,7 @@
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
-      <c r="M56" s="26"/>
+      <c r="M56" s="18"/>
       <c r="N56" s="26"/>
       <c r="O56" s="26"/>
       <c r="P56" s="26"/>
@@ -7324,11 +7320,11 @@
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="26"/>
-      <c r="O57" s="26"/>
-      <c r="P57" s="26"/>
-      <c r="Q57" s="26"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
       <c r="R57" s="1"/>
       <c r="S57" s="26"/>
       <c r="T57" s="26"/>
@@ -7337,7 +7333,6 @@
       <c r="W57" s="26"/>
     </row>
     <row r="58" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -7349,11 +7344,11 @@
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
-      <c r="M58" s="27"/>
-      <c r="N58" s="27"/>
-      <c r="O58" s="27"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
+      <c r="M58" s="26"/>
+      <c r="N58" s="26"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
       <c r="R58" s="1"/>
       <c r="S58" s="26"/>
       <c r="T58" s="26"/>
@@ -7362,6 +7357,7 @@
       <c r="W58" s="26"/>
     </row>
     <row r="59" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -7373,7 +7369,7 @@
       <c r="J59" s="18"/>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
-      <c r="M59" s="26"/>
+      <c r="M59" s="18"/>
       <c r="N59" s="26"/>
       <c r="O59" s="26"/>
       <c r="P59" s="26"/>
@@ -7398,11 +7394,11 @@
       <c r="J60" s="18"/>
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="26"/>
-      <c r="O60" s="26"/>
-      <c r="P60" s="26"/>
-      <c r="Q60" s="26"/>
+      <c r="M60" s="27"/>
+      <c r="N60" s="27"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
       <c r="R60" s="1"/>
       <c r="S60" s="26"/>
       <c r="T60" s="26"/>
@@ -7411,7 +7407,6 @@
       <c r="W60" s="26"/>
     </row>
     <row r="61" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -7423,11 +7418,11 @@
       <c r="J61" s="18"/>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="27"/>
-      <c r="O61" s="27"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
+      <c r="M61" s="26"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="26"/>
       <c r="R61" s="1"/>
       <c r="S61" s="26"/>
       <c r="T61" s="26"/>
@@ -7436,6 +7431,7 @@
       <c r="W61" s="26"/>
     </row>
     <row r="62" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -7447,7 +7443,7 @@
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="26"/>
+      <c r="M62" s="18"/>
       <c r="N62" s="26"/>
       <c r="O62" s="26"/>
       <c r="P62" s="26"/>
@@ -7472,11 +7468,11 @@
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="26"/>
-      <c r="O63" s="26"/>
-      <c r="P63" s="26"/>
-      <c r="Q63" s="26"/>
+      <c r="M63" s="27"/>
+      <c r="N63" s="27"/>
+      <c r="O63" s="27"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
       <c r="R63" s="1"/>
       <c r="S63" s="26"/>
       <c r="T63" s="26"/>
@@ -7485,7 +7481,6 @@
       <c r="W63" s="26"/>
     </row>
     <row r="64" spans="1:23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
@@ -7497,11 +7492,11 @@
       <c r="J64" s="18"/>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
-      <c r="M64" s="27"/>
-      <c r="N64" s="27"/>
-      <c r="O64" s="27"/>
-      <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
+      <c r="M64" s="26"/>
+      <c r="N64" s="26"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="26"/>
       <c r="R64" s="1"/>
       <c r="S64" s="26"/>
       <c r="T64" s="26"/>
@@ -7509,7 +7504,8 @@
       <c r="V64" s="26"/>
       <c r="W64" s="26"/>
     </row>
-    <row r="65" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="18"/>
       <c r="B65" s="18"/>
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
@@ -7521,17 +7517,19 @@
       <c r="J65" s="18"/>
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
-      <c r="M65" s="26"/>
+      <c r="M65" s="18"/>
       <c r="N65" s="26"/>
       <c r="O65" s="26"/>
       <c r="P65" s="26"/>
       <c r="Q65" s="26"/>
-      <c r="R65" s="1"/>
       <c r="S65" s="26"/>
       <c r="T65" s="26"/>
       <c r="U65" s="26"/>
       <c r="V65" s="26"/>
       <c r="W65" s="26"/>
+      <c r="X65" s="26"/>
+      <c r="Y65" s="26"/>
+      <c r="Z65" s="26"/>
     </row>
     <row r="66" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
@@ -7546,11 +7544,11 @@
       <c r="J66" s="18"/>
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
-      <c r="M66" s="18"/>
-      <c r="N66" s="26"/>
-      <c r="O66" s="26"/>
-      <c r="P66" s="26"/>
-      <c r="Q66" s="26"/>
+      <c r="M66" s="27"/>
+      <c r="N66" s="27"/>
+      <c r="O66" s="27"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
       <c r="S66" s="26"/>
       <c r="T66" s="26"/>
       <c r="U66" s="26"/>
@@ -7560,29 +7558,21 @@
       <c r="Y66" s="26"/>
       <c r="Z66" s="26"/>
     </row>
-    <row r="67" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="27"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
-      <c r="U67" s="26"/>
-      <c r="V67" s="26"/>
-      <c r="W67" s="26"/>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
       <c r="X67" s="26"/>
       <c r="Y67" s="26"/>
       <c r="Z67" s="26"/>
@@ -7629,7 +7619,7 @@
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
+      <c r="D70"/>
       <c r="E70"/>
       <c r="F70"/>
       <c r="G70"/>
@@ -7639,10 +7629,13 @@
       <c r="K70"/>
       <c r="L70"/>
       <c r="M70"/>
-      <c r="N70"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="R70" s="26"/>
+      <c r="S70" s="26"/>
+      <c r="W70" s="26"/>
       <c r="X70" s="26"/>
       <c r="Y70" s="26"/>
-      <c r="Z70" s="26"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71"/>
@@ -7658,10 +7651,6 @@
       <c r="K71"/>
       <c r="L71"/>
       <c r="M71"/>
-      <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
-      <c r="R71" s="26"/>
-      <c r="S71" s="26"/>
       <c r="W71" s="26"/>
       <c r="X71" s="26"/>
       <c r="Y71" s="26"/>
@@ -7720,65 +7709,60 @@
       <c r="X74" s="26"/>
       <c r="Y74" s="26"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A75"/>
-      <c r="B75"/>
+    <row r="75" spans="1:26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C75" s="34"/>
-      <c r="D75"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
-      <c r="J75"/>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-      <c r="W75" s="26"/>
-      <c r="X75" s="26"/>
-      <c r="Y75" s="26"/>
-    </row>
-    <row r="76" spans="1:26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K75" s="5"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+    </row>
+    <row r="76" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C76" s="34"/>
       <c r="K76" s="5"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
       <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
     </row>
-    <row r="77" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C77" s="34"/>
       <c r="K77" s="5"/>
-      <c r="N77" s="18"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
     </row>
-    <row r="78" spans="1:26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A78"/>
+      <c r="B78"/>
       <c r="C78" s="34"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
       <c r="K78" s="5"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-      <c r="T78" s="1"/>
-      <c r="U78" s="1"/>
-      <c r="V78" s="1"/>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79"/>
@@ -7806,33 +7790,30 @@
       <c r="J80"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81" s="34"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
-      <c r="J81"/>
+    <row r="81" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="5"/>
       <c r="K81" s="5"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
     </row>
     <row r="82" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
+      <c r="C82" s="34"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -7840,28 +7821,24 @@
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
     </row>
-    <row r="83" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
+    <row r="83" spans="1:25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="18"/>
       <c r="C83" s="34"/>
       <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
     </row>
-    <row r="84" spans="1:25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="18"/>
+    <row r="84" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C84" s="34"/>
-      <c r="N84" s="1"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="3"/>
-      <c r="Q84" s="1"/>
-      <c r="R84" s="1"/>
-      <c r="S84" s="1"/>
     </row>
     <row r="85" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C85" s="34"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="S85" s="1"/>
     </row>
     <row r="86" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C86" s="34"/>
@@ -7871,81 +7848,75 @@
     </row>
     <row r="87" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C87" s="34"/>
-      <c r="O87" s="3"/>
-      <c r="P87" s="3"/>
-      <c r="S87" s="1"/>
+      <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C88" s="34"/>
-      <c r="F88" s="1"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="S88" s="1"/>
     </row>
     <row r="89" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C89" s="34"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
-      <c r="S89" s="1"/>
+      <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C90" s="34"/>
-      <c r="F90" s="1"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="S90" s="1"/>
     </row>
     <row r="91" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C91" s="34"/>
-      <c r="O91" s="3"/>
-      <c r="P91" s="3"/>
-      <c r="S91" s="1"/>
+      <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C92" s="34"/>
       <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H92" s="1"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="S92" s="1"/>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A93"/>
+      <c r="B93"/>
       <c r="C93" s="34"/>
-      <c r="F93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="O93" s="3"/>
-      <c r="P93" s="3"/>
-      <c r="S93" s="1"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A94"/>
-      <c r="B94"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+      <c r="R93"/>
+      <c r="S93"/>
+      <c r="T93"/>
+      <c r="U93"/>
+      <c r="V93"/>
+      <c r="W93" s="26"/>
+      <c r="X93" s="26"/>
+      <c r="Y93" s="26"/>
+    </row>
+    <row r="94" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C94" s="34"/>
-      <c r="D94"/>
-      <c r="E94"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
-      <c r="N94"/>
-      <c r="O94"/>
-      <c r="P94"/>
-      <c r="Q94"/>
-      <c r="R94"/>
-      <c r="S94"/>
-      <c r="T94"/>
-      <c r="U94"/>
-      <c r="V94"/>
-      <c r="W94" s="26"/>
-      <c r="X94" s="26"/>
-      <c r="Y94" s="26"/>
-    </row>
-    <row r="95" spans="1:25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C95" s="34"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-      <c r="Q95" s="1"/>
-      <c r="R95" s="26"/>
-      <c r="S95" s="26"/>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C96" s="35"/>
-      <c r="I96" s="1"/>
-      <c r="K96" s="5"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="26"/>
+      <c r="S94" s="26"/>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C95" s="35"/>
+      <c r="I95" s="1"/>
+      <c r="K95" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8066,13 +8037,13 @@
     </row>
     <row r="6" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D6" s="34" t="b">
         <v>0</v>
@@ -8082,13 +8053,13 @@
     </row>
     <row r="7" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D7" s="34" t="b">
         <v>0</v>
@@ -8098,13 +8069,13 @@
     </row>
     <row r="8" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D8" s="34" t="b">
         <v>0</v>
@@ -8115,13 +8086,13 @@
     </row>
     <row r="9" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D9" s="34" t="b">
         <v>0</v>
@@ -8132,13 +8103,13 @@
     </row>
     <row r="10" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D10" s="34" t="b">
         <v>0</v>
@@ -8149,13 +8120,13 @@
     </row>
     <row r="11" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D11" s="34" t="b">
         <v>0</v>
@@ -8166,13 +8137,13 @@
     </row>
     <row r="12" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D12" s="34" t="b">
         <v>0</v>
@@ -8183,13 +8154,13 @@
     </row>
     <row r="13" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D13" s="34" t="b">
         <v>0</v>
@@ -8200,13 +8171,13 @@
     </row>
     <row r="14" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D14" s="34" t="b">
         <v>0</v>
@@ -8217,13 +8188,13 @@
     </row>
     <row r="15" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D15" s="34" t="b">
         <v>0</v>
@@ -8233,13 +8204,13 @@
     </row>
     <row r="16" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D16" s="34" t="b">
         <v>0</v>
@@ -8249,13 +8220,13 @@
     </row>
     <row r="17" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D17" s="34" t="b">
         <v>0</v>
@@ -8265,13 +8236,13 @@
     </row>
     <row r="18" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D18" s="34" t="b">
         <v>0</v>
@@ -8281,13 +8252,13 @@
     </row>
     <row r="19" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D19" s="34" t="b">
         <v>0</v>
@@ -8297,13 +8268,13 @@
     </row>
     <row r="20" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D20" s="34" t="b">
         <v>0</v>
@@ -8313,13 +8284,13 @@
     </row>
     <row r="21" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D21" s="34" t="b">
         <v>0</v>
@@ -8330,13 +8301,13 @@
     </row>
     <row r="22" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D22" s="34" t="b">
         <v>0</v>
@@ -8347,13 +8318,13 @@
     </row>
     <row r="23" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D23" s="34" t="b">
         <v>0</v>
@@ -8363,13 +8334,13 @@
     </row>
     <row r="24" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D24" s="34" t="b">
         <v>0</v>
@@ -8379,13 +8350,13 @@
     </row>
     <row r="25" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D25" s="34" t="b">
         <v>0</v>
@@ -8395,13 +8366,13 @@
     </row>
     <row r="26" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D26" s="34" t="b">
         <v>0</v>
@@ -8412,13 +8383,13 @@
     </row>
     <row r="27" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D27" s="34" t="b">
         <v>0</v>
@@ -8429,13 +8400,13 @@
     </row>
     <row r="28" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D28" s="34" t="b">
         <v>0</v>
@@ -8446,13 +8417,13 @@
     </row>
     <row r="29" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D29" s="34" t="b">
         <v>0</v>

</xml_diff>